<commit_message>
Add docs of architect
</commit_message>
<xml_diff>
--- a/Docs/LearningPath_Track.xlsx
+++ b/Docs/LearningPath_Track.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Learning\Architect\Git\architectgit\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1AEF76E-5F39-4713-AEA3-25410308D9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6405B2-5ACB-4BA3-A679-BCD01AF593FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="3" xr2:uid="{A27247F4-4302-493B-8584-F190D66B2294}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="4" xr2:uid="{A27247F4-4302-493B-8584-F190D66B2294}"/>
   </bookViews>
   <sheets>
     <sheet name="UI" sheetId="1" r:id="rId1"/>
     <sheet name="Mobile App" sheetId="2" r:id="rId2"/>
-    <sheet name="System Desing" sheetId="3" r:id="rId3"/>
+    <sheet name="System Design" sheetId="3" r:id="rId3"/>
     <sheet name="DSA" sheetId="4" r:id="rId4"/>
     <sheet name="Architecture Design" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t xml:space="preserve">UI </t>
   </si>
@@ -71,9 +71,6 @@
     <t>Pre Sales</t>
   </si>
   <si>
-    <t>After Pre sales</t>
-  </si>
-  <si>
     <t>Sl.No</t>
   </si>
   <si>
@@ -93,13 +90,40 @@
   </si>
   <si>
     <t>Analysis of Algorithms</t>
+  </si>
+  <si>
+    <t>After Pre Sales</t>
+  </si>
+  <si>
+    <t>Introduction and Goals</t>
+  </si>
+  <si>
+    <t>Architecture Constraints</t>
+  </si>
+  <si>
+    <t>Business Context</t>
+  </si>
+  <si>
+    <t>Technical Context</t>
+  </si>
+  <si>
+    <t>Building Block View</t>
+  </si>
+  <si>
+    <t>Level -1</t>
+  </si>
+  <si>
+    <t>Level -2</t>
+  </si>
+  <si>
+    <t>Level -3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +135,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF4F81BD"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF4F81BD"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,12 +176,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -287,14 +336,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEEBC360-3F78-4073-ADDD-0B262065476F}" name="Table1" displayName="Table1" ref="A2:E4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{FEEBC360-3F78-4073-ADDD-0B262065476F}" name="Table1" displayName="Table1" ref="A2:E4" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A2:E4" xr:uid="{FEEBC360-3F78-4073-ADDD-0B262065476F}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{05EF6D79-3E44-4515-8BB9-6E53AB1943CA}" name="Sl.No" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D1CB603E-1A05-4D69-BAB4-C8A386E43E87}" name="Topic" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{15D63996-1EF6-4F0F-B47A-875A7F2C94C3}" name="Sub Topic " dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{EF2FB37D-D0FA-4915-9D68-6ED870527814}" name="Status" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{1F1BE6D2-6354-4B3E-8586-B15A2144D13D}" name="Date" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{05EF6D79-3E44-4515-8BB9-6E53AB1943CA}" name="Sl.No" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{D1CB603E-1A05-4D69-BAB4-C8A386E43E87}" name="Topic" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{15D63996-1EF6-4F0F-B47A-875A7F2C94C3}" name="Sub Topic " dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{EF2FB37D-D0FA-4915-9D68-6ED870527814}" name="Status" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{1F1BE6D2-6354-4B3E-8586-B15A2144D13D}" name="Date" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -615,6 +664,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_GPT</we:customFunctionIds>
@@ -733,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{860F76F6-7467-495B-815C-026DDAC3D7E0}">
   <dimension ref="A2:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -744,50 +796,50 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -800,40 +852,81 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E07AFE9-7454-492E-A946-18D63416197D}">
-  <dimension ref="B6:C13"/>
+  <dimension ref="B6:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-      <c r="C7" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
-      <c r="C8" t="s">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2"/>
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>13</v>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="2:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>